<commit_message>
arquivos ultima execucao sp
</commit_message>
<xml_diff>
--- a/inst/tabelas_depara/taurus_regra_1.xlsx
+++ b/inst/tabelas_depara/taurus_regra_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wamorim/Documents/institutosoudapaz/isdp.armas/inst/tabelas_depara/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandopoliano/projetos.R/isdp.armas/inst/tabelas_depara/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57ED6DED-E764-1741-87B6-D3446B46CB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEDF2E5-AF5D-1947-AFD6-A723E88A88E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9620" yWindow="3600" windowWidth="27640" windowHeight="16940" xr2:uid="{4887C932-7DA5-6E45-B977-00DF947F2A32}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" xr2:uid="{4887C932-7DA5-6E45-B977-00DF947F2A32}"/>
   </bookViews>
   <sheets>
     <sheet name="regra_1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +78,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,9 +127,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -160,7 +167,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -266,7 +273,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -408,7 +415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -416,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74233B74-2AFA-9B47-A95E-1544A8E95094}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E38" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,7 +437,7 @@
     <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -457,8 +464,9 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -472,7 +480,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -486,7 +494,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -500,7 +508,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -514,7 +522,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -528,7 +536,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -542,7 +550,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -556,7 +564,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -570,7 +578,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -584,7 +592,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -598,7 +606,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -612,7 +620,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -626,7 +634,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -640,7 +648,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>

</xml_diff>